<commit_message>
Update use case descriptions (step by step breakdown).xlsx
</commit_message>
<xml_diff>
--- a/use case descriptions (step by step breakdown).xlsx
+++ b/use case descriptions (step by step breakdown).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F50129D-3AFE-4369-8652-A14EF8908874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B14362F-F318-4A41-81FE-68C80A2D3EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Use case description: 대여소 검색</t>
   </si>
@@ -42,94 +42,103 @@
     <t>System Response</t>
   </si>
   <si>
-    <t>1. 회원이 시스템에 로그인한다.</t>
-  </si>
-  <si>
-    <t>2. 대여소 검색 화면을 표시한다.</t>
-  </si>
-  <si>
-    <t>3. 회원이 대여소 이름(또는 키워드)을 입력한다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. 해당 조건에 맞는 대여소 리스트를 출력한다.
+    <t>1. None</t>
+  </si>
+  <si>
+    <t>2. 로그인, 회원 가입 메뉴를 띄운다.</t>
+  </si>
+  <si>
+    <t>3. 로그인 메뉴를 누른다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. 로그인 화면을 띄운다.
 </t>
   </si>
   <si>
+    <t>5. 사용자 ID와 비밀번호를 입력한다.</t>
+  </si>
+  <si>
+    <t>6. 회원용 메뉴를 띄운다.</t>
+  </si>
+  <si>
+    <t>7. 회원이 시스템에 로그인한다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	8. 시스템은 회원 전용 기능을 표시한다.</t>
+  </si>
+  <si>
+    <t>9. 대여소 검색 메뉴를 선택한다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. 대여소 검색 창이 출력된다.
+</t>
+  </si>
+  <si>
+    <t>11. 대여소 이름 또는 키워드를 입력한다.</t>
+  </si>
+  <si>
+    <t>12. 조건에 맞는 대여소 리스트가 출력된다.</t>
+  </si>
+  <si>
     <t>Use case description: 대여소 상세정보 조회</t>
   </si>
   <si>
-    <t>1. 회원이 대여소 검색 결과 리스트를 확인한다.</t>
-  </si>
-  <si>
-    <t>2. 시스템은 각 대여소에 대한 기본 정보를 표시한다.</t>
-  </si>
-  <si>
-    <t>3. 회원이 특정 대여소를 선택한다.</t>
-  </si>
-  <si>
-    <t>4. 선택한 대여소의 상세정보(대여소 이름, 대여소 위치, 사용 가능 자전거 목록 등)를 보여준다.</t>
+    <t>7. 회원이 대여소 검색 결과에서 특정 항목을 선택한다.</t>
+  </si>
+  <si>
+    <t>8. 해당 대여소의 상세정보(대여소 이름, 대여소 위치, 사용 가능 자전거 목록 등)를 표시한다.</t>
+  </si>
+  <si>
+    <t>9. 해당 대여소의 상세정보를 확인한다.</t>
+  </si>
+  <si>
+    <t>10. 자전거가 0대일 경우, 예약 대기 신청 옵션을 활성화한다.</t>
+  </si>
+  <si>
+    <t>Extension
+Step 10 이후, 자전거가 없을 경우 자전거 예약 대기 신청을 할 수 있다.</t>
+  </si>
+  <si>
+    <t>Use case description: 자전거 예약 대기 신청</t>
+  </si>
+  <si>
+    <t>7. 회원이 상세정보 화면에서 자전거가 모두 대여 중임을 확인한다.</t>
+  </si>
+  <si>
+    <t>8. 예약 대기 버튼이 표시된다.</t>
+  </si>
+  <si>
+    <t>9. 회원이 예약 대기 신청을 클릭한다.</t>
+  </si>
+  <si>
+    <t>10. 회원을 예약 대기 목록에 추가한다.</t>
+  </si>
+  <si>
+    <t>11. 문자 알림 전송 서비스에게 예약 대기 완료 알림을 요청한다.</t>
+  </si>
+  <si>
+    <t>12. 문자 알림 전송 서비스가 회원에게 문자 메시지를 보낸다.</t>
   </si>
   <si>
     <t>Use case description: 자전거 즉시 대여</t>
   </si>
   <si>
-    <t>1. 회원이 대여소 상세 화면에서 사용 가능한 자전거를 선택한다.</t>
-  </si>
-  <si>
-    <t>2. 시스템은 자전거 상태(사용 가능 여부)를 확인한다.</t>
-  </si>
-  <si>
-    <t>3. 회원이 대여 버튼을 클릭한다.</t>
-  </si>
-  <si>
-    <t>4. 시스템은 대여를 처리하고 자전거 상태를 “대여 중”으로 변경한다.</t>
-  </si>
-  <si>
-    <t>5. &lt;&lt;extend&gt;&gt; 대여 완료 문자 알림 전송 Use Case 실행됨.</t>
-  </si>
-  <si>
-    <t>Use case description: 자전거 예약 대기 신청</t>
-  </si>
-  <si>
-    <t>1. 회원이 대여소 상세 화면에서 자전거가 모두 대여 중인 것을 확인한다.</t>
-  </si>
-  <si>
-    <t>2. 시스템은 예약 대기 버튼을 활성화한다.</t>
-  </si>
-  <si>
-    <t>3. 회원이 예약 대기를 신청한다.</t>
-  </si>
-  <si>
-    <t>4. 시스템은 대기 명단에 회원을 등록한다.</t>
-  </si>
-  <si>
-    <t>5. &lt;&lt;extend&gt;&gt; 예약 대기 완료 문자 알림 전송 Use Case 실행됨.</t>
-  </si>
-  <si>
-    <t>Use case description: 대여 완료 문자 알림 전송</t>
-  </si>
-  <si>
-    <t>1. 없음 (자전거 즉시 대여 완료 시 자동 실행)</t>
-  </si>
-  <si>
-    <t>2. 문자 알림 전송 서비스에 대여 완료 알림 요청을 전송한다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. 문자 알림 전송 서비스가 회원에게 대여 완료 문자 메시지를 보낸다.
-</t>
-  </si>
-  <si>
-    <t>Use case description: 예약 대기 완료 문자 알림 전송</t>
-  </si>
-  <si>
-    <t>1. 없음 (예약 대기 신청 완료 시 자동 실행)</t>
-  </si>
-  <si>
-    <t>2. 문자 알림 전송 서비스에 예약 대기 알림 요청을 전송한다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. 문자 알림 전송 서비스가 회원에게 예약 대기 완료 문자 메시지를 보낸다.
-</t>
+    <t>7. 회원이 대여소 상세정보에서 사용 가능한 자전거를 선택한다.</t>
+  </si>
+  <si>
+    <t>8. 시스템은 자전거 상태(사용 가능 여부)를 확인한다.</t>
+  </si>
+  <si>
+    <t>9. 즉시 대여 버튼을 클릭한다.</t>
+  </si>
+  <si>
+    <t>10. 시스템은 대여를 처리하고 자전거 상태를 “대여 중”으로 변경한다.</t>
+  </si>
+  <si>
+    <t>Use case description: 문자 알림 전송 서비스 (외부 서비스)</t>
+  </si>
+  <si>
+    <t>2. 문자 알림 전송 서비스는 요청을 받아 회원에게 알림 메시지를 발송한다.</t>
   </si>
 </sst>
 </file>
@@ -181,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -189,14 +198,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -546,10 +564,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="3"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3">
@@ -562,133 +580,131 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="33">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="26.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="33">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="26.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="33">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="33">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="26.25">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="33">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="33">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26.25">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="33">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:2" s="7" customFormat="1" ht="33" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" ht="26.25">
+      <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="26.25">
-      <c r="A19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
@@ -698,56 +714,162 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="33">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19.5" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="33">
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="33">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="26.25">
-      <c r="A23" s="5" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" ht="26.25">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="4" t="s">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="33">
-      <c r="A25" s="3" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="33">
+      <c r="A34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="33">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20.25" customHeight="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:2" ht="26.25">
+      <c r="A39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
05.08 use case description 수정
</commit_message>
<xml_diff>
--- a/use case descriptions (step by step breakdown).xlsx
+++ b/use case descriptions (step by step breakdown).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B14362F-F318-4A41-81FE-68C80A2D3EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF283DC5-F996-4D34-890B-79C352391DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Use case description: 대여소 검색</t>
   </si>
@@ -61,23 +61,17 @@
     <t>6. 회원용 메뉴를 띄운다.</t>
   </si>
   <si>
-    <t>7. 회원이 시스템에 로그인한다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	8. 시스템은 회원 전용 기능을 표시한다.</t>
-  </si>
-  <si>
-    <t>9. 대여소 검색 메뉴를 선택한다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. 대여소 검색 창이 출력된다.
+    <t>7. 대여소 검색 메뉴를 선택한다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. 대여소 검색 창이 출력된다.
 </t>
   </si>
   <si>
-    <t>11. 대여소 이름 또는 키워드를 입력한다.</t>
-  </si>
-  <si>
-    <t>12. 조건에 맞는 대여소 리스트가 출력된다.</t>
+    <t>9. 대여소 이름 또는 키워드를 입력한다.</t>
+  </si>
+  <si>
+    <t>10. 조건에 맞는 대여소 리스트가 출력된다.</t>
   </si>
   <si>
     <t>Use case description: 대여소 상세정보 조회</t>
@@ -86,53 +80,38 @@
     <t>7. 회원이 대여소 검색 결과에서 특정 항목을 선택한다.</t>
   </si>
   <si>
-    <t>8. 해당 대여소의 상세정보(대여소 이름, 대여소 위치, 사용 가능 자전거 목록 등)를 표시한다.</t>
-  </si>
-  <si>
-    <t>9. 해당 대여소의 상세정보를 확인한다.</t>
-  </si>
-  <si>
-    <t>10. 자전거가 0대일 경우, 예약 대기 신청 옵션을 활성화한다.</t>
+    <t>8. 해당 대여소의 상세정보(대여소 이름, 대여소 위치, 사용 가능 자전거 목록 등)를 표시하고 자전거가 0대일 경우, 예약 대기 신청 옵션을 활성화한다.</t>
+  </si>
+  <si>
+    <t>9. 원하는 자전거가 없을 경우 해당 자전거를 선택해서 예약 대기 신청을 버튼을 클릭한다.</t>
+  </si>
+  <si>
+    <t>10. 회원을 예약 대기 목록에 추가한다.</t>
+  </si>
+  <si>
+    <t>11. 문자 알림 전송 서비스에게 예약 대기 완료 알림을 요청한다.</t>
+  </si>
+  <si>
+    <t>12. 문자 알림 전송 서비스가 회원에게 문자 메시지를 보낸다.</t>
   </si>
   <si>
     <t>Extension
-Step 10 이후, 자전거가 없을 경우 자전거 예약 대기 신청을 할 수 있다.</t>
-  </si>
-  <si>
-    <t>Use case description: 자전거 예약 대기 신청</t>
-  </si>
-  <si>
-    <t>7. 회원이 상세정보 화면에서 자전거가 모두 대여 중임을 확인한다.</t>
-  </si>
-  <si>
-    <t>8. 예약 대기 버튼이 표시된다.</t>
-  </si>
-  <si>
-    <t>9. 회원이 예약 대기 신청을 클릭한다.</t>
-  </si>
-  <si>
-    <t>10. 회원을 예약 대기 목록에 추가한다.</t>
-  </si>
-  <si>
-    <t>11. 문자 알림 전송 서비스에게 예약 대기 완료 알림을 요청한다.</t>
-  </si>
-  <si>
-    <t>12. 문자 알림 전송 서비스가 회원에게 문자 메시지를 보낸다.</t>
+Step 8 이후, 자전거가 없을 경우 자전거 예약 대기 신청을 할 수 있다.</t>
   </si>
   <si>
     <t>Use case description: 자전거 즉시 대여</t>
   </si>
   <si>
-    <t>7. 회원이 대여소 상세정보에서 사용 가능한 자전거를 선택한다.</t>
-  </si>
-  <si>
-    <t>8. 시스템은 자전거 상태(사용 가능 여부)를 확인한다.</t>
-  </si>
-  <si>
-    <t>9. 즉시 대여 버튼을 클릭한다.</t>
-  </si>
-  <si>
-    <t>10. 시스템은 대여를 처리하고 자전거 상태를 “대여 중”으로 변경한다.</t>
+    <t>7. 회원이 대여소 상세정보에서 사용 가능한 자전거를 선택하고 즉시 대여 버튼을 클릭한다.</t>
+  </si>
+  <si>
+    <t>8. 시스템은 대여를 처리하고 자전거 상태를 “대여 중”으로 변경한다.</t>
+  </si>
+  <si>
+    <t>9. 문자 알림 전송 서비스에게 예약 대기 완료 알림을 요청한다.</t>
+  </si>
+  <si>
+    <t>10. 문자 알림 전송 서비스가 회원에게 문자 메시지를 보낸다.</t>
   </si>
   <si>
     <t>Use case description: 문자 알림 전송 서비스 (외부 서비스)</t>
@@ -190,13 +169,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -550,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -571,305 +553,224 @@
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="33">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:3" ht="33">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="33">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
+    <row r="9" spans="1:3" ht="48.75" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="33">
+      <c r="A12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="33">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" ht="26.25">
-      <c r="A10" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="33">
-      <c r="A15" s="5" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="53.25" customHeight="1">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:2" s="8" customFormat="1" ht="33" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="7" customFormat="1" ht="33" customHeight="1">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:2" ht="49.5" customHeight="1">
+      <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" ht="26.25">
-      <c r="A19" s="3" t="s">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" ht="26.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="48.75" customHeight="1">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19.5" customHeight="1">
+      <c r="A22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="19.5" customHeight="1">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:2" ht="33">
+      <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="33">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:2" ht="49.5">
+      <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-    </row>
-    <row r="29" spans="1:2" ht="26.25">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" ht="48.75" customHeight="1">
+      <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="18" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="33">
-      <c r="A34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5" t="s">
+      <c r="B31" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" ht="26.25">
-      <c r="A39" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    <row r="32" spans="1:2" ht="18" customHeight="1"/>
+    <row r="36" ht="20.25" customHeight="1"/>
+    <row r="39" ht="26.25" customHeight="1"/>
+    <row r="40" ht="73.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A19:B19"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>